<commit_message>
added case assembly information.
</commit_message>
<xml_diff>
--- a/操作ボタン説明.xlsx
+++ b/操作ボタン説明.xlsx
@@ -13,9 +13,183 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>【モード/メニュー】</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>２．時間設定</t>
+    <rPh sb="2" eb="4">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>３．日付設定</t>
+    <rPh sb="2" eb="4">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>１．音楽再生</t>
+    <rPh sb="2" eb="4">
+      <t>オンガク</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>サイセイ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>４．チャイム機能　ON</t>
+    <rPh sb="6" eb="8">
+      <t>キノウ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>５．チャイム機能　OFF</t>
+    <rPh sb="6" eb="8">
+      <t>キノウ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>【時刻設定方法】</t>
+    <rPh sb="1" eb="3">
+      <t>ジコク</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ホウホウ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>１．モードセレクトを1回押す</t>
+    <rPh sb="11" eb="12">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>オ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>２．UPボタンを押す</t>
+    <rPh sb="8" eb="9">
+      <t>オ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>４．時間を変更しモードセレクトを押す。</t>
+    <rPh sb="2" eb="4">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>オ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>５．分を変更しモードセレクトを押す。</t>
+    <rPh sb="2" eb="3">
+      <t>フン</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>オ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>※UP/DOWNボタンを長押しすると、数字が早く動きます。</t>
+    <rPh sb="12" eb="14">
+      <t>ナガオ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>スウジ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ハヤ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ウゴ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>６．Time Set? と表示されるので、モードセレクトを押す。</t>
+    <rPh sb="13" eb="15">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>オ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>３．Set the Time　と表示されるので、モードセレクトを押す。</t>
+    <rPh sb="16" eb="18">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>オ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>以上です。　※日付も同様です。</t>
+    <rPh sb="0" eb="2">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ドウヨウ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>■操作ボタン説明</t>
+    <rPh sb="1" eb="3">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>※メニューボタンを一回押して、続けて、UPボタンを押してください。　メニューが切り替わります。</t>
+  </si>
+  <si>
+    <t>　UPボタンを1回押す毎に、時間設定→日付設定→チャイムON→チャイムOFF とメニューが切り替わります。</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +350,15 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -608,11 +791,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -678,7 +864,7 @@
       <xdr:col>40</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1019,7 +1205,23 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>・モードセレクト</a:t>
+            <a:t>・モード</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>メニュー</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200" b="1">
             <a:solidFill>
@@ -1035,7 +1237,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>・時間設定確定</a:t>
+            <a:t>・設定確定</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1610,17 +1812,108 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="F3:K75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AO46" sqref="AO46"/>
+      <selection activeCell="AV60" sqref="AV60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="16384" width="2.875" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="6:6" ht="14.25">
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="9:10">
+      <c r="I56" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="9:10">
+      <c r="J57" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="9:10">
+      <c r="J58" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="9:10">
+      <c r="J59" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="9:10">
+      <c r="J60" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="9:10">
+      <c r="J61" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="9:10">
+      <c r="J62" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="9:10">
+      <c r="J63" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="9:11">
+      <c r="I67" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="9:11">
+      <c r="J68" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="9:11">
+      <c r="J69" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="9:11">
+      <c r="J70" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="9:11">
+      <c r="J71" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="9:11">
+      <c r="J72" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="9:11">
+      <c r="K73" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="9:11">
+      <c r="J74" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="9:11">
+      <c r="K75" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <sortState ref="A48:D72">
     <sortCondition ref="B48:B72"/>
     <sortCondition ref="C48:C72"/>

</xml_diff>